<commit_message>
admin userinfo and order detail
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HK2_3\Web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITUS\Nam III\HKII\Web\Project\Shop\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7656"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="112">
   <si>
     <t>ID</t>
   </si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t>Hàn Quốc</t>
+  </si>
+  <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
   </si>
 </sst>
 </file>
@@ -735,26 +741,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="1"/>
-    <col min="2" max="2" width="24.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1"/>
-    <col min="6" max="6" width="24.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="1"/>
-    <col min="8" max="9" width="20.85546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="13.7109375" style="1"/>
+    <col min="1" max="1" width="13.6640625" style="1"/>
+    <col min="2" max="2" width="24.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="1"/>
+    <col min="6" max="6" width="24.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="1"/>
+    <col min="8" max="9" width="20.88671875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="13.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,8 +791,14 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="100.5" customHeight="1">
+      <c r="K1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="100.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -818,7 +830,7 @@
         <v>1835</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="70.5" customHeight="1">
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="70.5" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -850,7 +862,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="81" customHeight="1">
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="81" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
@@ -882,7 +894,7 @@
         <v>1948</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" ht="105" customHeight="1">
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="105" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
@@ -914,7 +926,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="90">
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="86.4">
       <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
@@ -946,7 +958,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="75">
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="72">
       <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
@@ -978,7 +990,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="75">
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="57.6">
       <c r="A8" s="2" t="s">
         <v>47</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>1921</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" ht="75">
+    <row r="9" spans="1:12" s="4" customFormat="1" ht="72">
       <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
@@ -1042,7 +1054,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="90">
+    <row r="10" spans="1:12" s="2" customFormat="1" ht="86.4">
       <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
@@ -1074,7 +1086,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" ht="90">
+    <row r="11" spans="1:12" s="2" customFormat="1" ht="72">
       <c r="A11" s="2" t="s">
         <v>50</v>
       </c>
@@ -1106,7 +1118,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" ht="142.5">
+    <row r="12" spans="1:12" s="2" customFormat="1" ht="138">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>1851</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="2" customFormat="1" ht="85.5">
+    <row r="13" spans="1:12" s="2" customFormat="1" ht="69">
       <c r="A13" s="2" t="s">
         <v>52</v>
       </c>
@@ -1170,7 +1182,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" ht="60">
+    <row r="14" spans="1:12" s="2" customFormat="1" ht="43.2">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
@@ -1202,7 +1214,7 @@
         <v>1895</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="4" customFormat="1" ht="99.75">
+    <row r="15" spans="1:12" s="4" customFormat="1" ht="96.6">
       <c r="A15" s="4" t="s">
         <v>54</v>
       </c>
@@ -1234,7 +1246,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" ht="142.5">
+    <row r="16" spans="1:12" s="2" customFormat="1" ht="124.2">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -1266,7 +1278,7 @@
         <v>1927</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="2" customFormat="1" ht="150">
+    <row r="17" spans="1:10" s="2" customFormat="1" ht="129.6">
       <c r="A17" s="2" t="s">
         <v>56</v>
       </c>
@@ -1330,7 +1342,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="2" customFormat="1" ht="60">
+    <row r="19" spans="1:10" s="2" customFormat="1" ht="43.2">
       <c r="A19" s="2" t="s">
         <v>61</v>
       </c>
@@ -1394,7 +1406,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="2" customFormat="1" ht="45">
+    <row r="21" spans="1:10" s="2" customFormat="1" ht="43.2">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>

</xml_diff>